<commit_message>
Change Stack and Queue Page Factory and Feature file , ConfigReader and Excel Reader
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/dsAlgoData.xlsx
+++ b/src/test/resources/TestData/dsAlgoData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{97D4A131-0B15-4F28-AD94-B138F262E06B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\TestBDD\NinjaTester\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516B0B95-433C-4BA7-B8E5-F9D85F601B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36135" yWindow="2910" windowWidth="14400" windowHeight="8235" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Register" sheetId="1" r:id="rId1"/>
@@ -13,25 +18,11 @@
     <sheet name="PythonCode" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:J19"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="27">
   <si>
     <t>username</t>
   </si>
@@ -159,12 +150,18 @@
   <si>
     <t>[4, 9, 9, 49, 121]</t>
   </si>
+  <si>
+    <t>NinjaTester</t>
+  </si>
+  <si>
+    <t>Welcome@123</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +181,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -209,9 +214,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -220,12 +226,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
   </cellStyles>
@@ -506,10 +513,10 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -549,10 +556,10 @@
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -591,10 +598,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="21.19921875" customWidth="1"/>
-    <col min="2" max="2" width="17.1328125" customWidth="1"/>
+    <col min="1" max="1" width="21.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -607,13 +614,16 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1E58A908-E844-4D4E-873E-9831364FAA03}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -624,11 +634,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="104.53125" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1328125" customWidth="1"/>
+    <col min="1" max="1" width="104.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" customWidth="1"/>
+    <col min="3" max="3" width="19.08984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>